<commit_message>
Deploying to gh-pages from @ Alvearie/alvearie-fhir-ig@b1dc07e60a9d87cd58c4b4b4c87c34a90f825dde 🚀
</commit_message>
<xml_diff>
--- a/1.0.0/StructureDefinition-claim-status.xlsx
+++ b/1.0.0/StructureDefinition-claim-status.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AJ$7</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="73">
   <si>
     <t>Path</t>
   </si>
@@ -225,8 +225,24 @@
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
   </si>
   <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>closed</t>
+  </si>
+  <si>
     <t xml:space="preserve">ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
 </t>
+  </si>
+  <si>
+    <t>valueCodeableConcept</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>https://x12.org/codes/claim-status-codes</t>
   </si>
 </sst>
 </file>
@@ -375,7 +391,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -385,7 +401,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="19.59375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="22.25" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="8.95703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.7734375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.9453125" customWidth="true" bestFit="true"/>
@@ -408,7 +424,7 @@
     <col min="22" max="22" width="19.03125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="18.85546875" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="21.5703125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="19.625" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="38.53515625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="6.34765625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="22.71484375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="42.03125" customWidth="true" bestFit="true"/>
@@ -1004,16 +1020,14 @@
         <v>37</v>
       </c>
       <c r="AA6" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="AB6" t="s" s="2">
-        <v>37</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="AB6" s="2"/>
       <c r="AC6" t="s" s="2">
         <v>37</v>
       </c>
       <c r="AD6" t="s" s="2">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="AE6" t="s" s="2">
         <v>63</v>
@@ -1028,14 +1042,114 @@
         <v>37</v>
       </c>
       <c r="AI6" t="s" s="2">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="AJ6" t="s" s="2">
         <v>62</v>
       </c>
     </row>
+    <row r="7" hidden="true">
+      <c r="A7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="I7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J7" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="K7" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="L7" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="R7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="S7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="T7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="U7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="V7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="W7" t="s" s="2">
+        <v>71</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="Z7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AA7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AB7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AC7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AD7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AE7" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="AF7" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="AG7" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH7" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="AI7" t="s" s="2">
+        <v>69</v>
+      </c>
+      <c r="AJ7" t="s" s="2">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AJ6">
+  <autoFilter ref="A1:AJ7">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -1045,7 +1159,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI5">
+  <conditionalFormatting sqref="A2:AI6">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>